<commit_message>
projet BTS 1 et 2
</commit_message>
<xml_diff>
--- a/assets/document/04 - Tableau de synthèse - Epreuve E4.xlsx
+++ b/assets/document/04 - Tableau de synthèse - Epreuve E4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Johan\GitHub\mes repertoire\Portfolio\assets\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508A68FC-4EE6-41B9-8199-A23085817395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065349FE-0C77-4B6C-A7BF-223CA318142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,7 +257,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -617,6 +617,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -625,7 +647,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -687,15 +709,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -729,29 +775,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1133,8 +1159,8 @@
   </sheetPr>
   <dimension ref="A1:AQ80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1147,56 +1173,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="41" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="29"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1208,22 +1234,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="38" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1246,8 +1272,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="19" t="s">
         <v>9</v>
       </c>
@@ -1263,10 +1289,10 @@
       <c r="G7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I7"/>
+      <c r="I7" s="43"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -1303,16 +1329,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1709,12 +1735,20 @@
         <v>34</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="14"/>
+      <c r="C16" s="20" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G16" s="20" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H16" s="15" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1756,12 +1790,20 @@
         <v>35</v>
       </c>
       <c r="B17" s="8"/>
-      <c r="C17" s="14"/>
+      <c r="C17" s="20" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G17" s="20" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H17" s="15" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1799,16 +1841,16 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -2161,16 +2203,16 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="29"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2615,11 +2657,6 @@
     <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2627,6 +2664,11 @@
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>